<commit_message>
regenerated version 1.0.0 pages
</commit_message>
<xml_diff>
--- a/v1.0.0/CodeSystem-VRM-MessageHeaderURI-cs.xlsx
+++ b/v1.0.0/CodeSystem-VRM-MessageHeaderURI-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-12-28T11:01:10-05:00</t>
+    <t>2023-12-28T12:14:20-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>